<commit_message>
Edición esqueleto guión CN_03_04_CO
Edición del esqueleto de guión de CN_03_04_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado03/guion04/EsqueletoGuion_CN_03_04_CO.xlsx
+++ b/fuentes/contenidos/grado03/guion04/EsqueletoGuion_CN_03_04_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="2"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="91">
   <si>
     <t>FICHA</t>
   </si>
@@ -173,6 +173,132 @@
   </si>
   <si>
     <t>Identificación de los recursos naturales renovables</t>
+  </si>
+  <si>
+    <t>Texto</t>
+  </si>
+  <si>
+    <t>Foto</t>
+  </si>
+  <si>
+    <t>Recuerda</t>
+  </si>
+  <si>
+    <t>Profundiza</t>
+  </si>
+  <si>
+    <t>Practica</t>
+  </si>
+  <si>
+    <t>Consolidación</t>
+  </si>
+  <si>
+    <t>El aire</t>
+  </si>
+  <si>
+    <t>La composición del aire</t>
+  </si>
+  <si>
+    <t>Destacado</t>
+  </si>
+  <si>
+    <t>Los beneficios del aire</t>
+  </si>
+  <si>
+    <t>Daños causados al aire por el ser humano</t>
+  </si>
+  <si>
+    <t>Contaminación por gases provenientes de vehículos</t>
+  </si>
+  <si>
+    <t>Contaminación por desechos industriales</t>
+  </si>
+  <si>
+    <t>Contaminación por quema de selvas y bosques</t>
+  </si>
+  <si>
+    <t>Conservación del aire</t>
+  </si>
+  <si>
+    <t>El agua</t>
+  </si>
+  <si>
+    <t>Los beneficios del agua</t>
+  </si>
+  <si>
+    <t>Daños causados al agua por parte del ser humano</t>
+  </si>
+  <si>
+    <t>Contaminación por basuras</t>
+  </si>
+  <si>
+    <t>Contaminación por actividades humanas</t>
+  </si>
+  <si>
+    <t>Conservación del agua</t>
+  </si>
+  <si>
+    <t>El suelo</t>
+  </si>
+  <si>
+    <t>Los tipos de suelo</t>
+  </si>
+  <si>
+    <t>Suelos fértiles y áridos</t>
+  </si>
+  <si>
+    <t>Los beneficios del suelo</t>
+  </si>
+  <si>
+    <t>Daños causados al suelo por parte del ser humano</t>
+  </si>
+  <si>
+    <t>Contaminación por basuras y desechos industriales</t>
+  </si>
+  <si>
+    <t>Contaminación por insecticidas y fertilizantes</t>
+  </si>
+  <si>
+    <t>La erosión</t>
+  </si>
+  <si>
+    <t>Conservación de los suelos</t>
+  </si>
+  <si>
+    <t>La Flora</t>
+  </si>
+  <si>
+    <t>Los beneficios de la flora</t>
+  </si>
+  <si>
+    <t>Daños causados a la flora por parte del ser humano</t>
+  </si>
+  <si>
+    <t>La conservación de la flora</t>
+  </si>
+  <si>
+    <t>La fauna</t>
+  </si>
+  <si>
+    <t>Los beneficios de la fauna</t>
+  </si>
+  <si>
+    <t>La conservación de la fauna</t>
+  </si>
+  <si>
+    <t>Competencias</t>
+  </si>
+  <si>
+    <t>Fin de unidad</t>
+  </si>
+  <si>
+    <t>Mapa Conceptual</t>
+  </si>
+  <si>
+    <t>Evaluación</t>
+  </si>
+  <si>
+    <t>El deterioro que genera el ser humano a la fauna</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1545,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1848,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -1841,7 +1967,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,7 +2147,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>27</v>
@@ -2135,10 +2261,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2147,7 +2274,9 @@
     <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="48.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="64.140625" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2182,8 +2311,15 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -2191,8 +2327,15 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -2200,8 +2343,15 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -2209,8 +2359,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -2218,8 +2375,15 @@
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -2227,35 +2391,80 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -2263,8 +2472,15 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -2272,26 +2488,59 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -2299,8 +2548,15 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2308,98 +2564,1268 @@
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="5"/>
     </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H48" t="s">
+        <v>32</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H62" t="s">
+        <v>33</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H65" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H69" t="s">
+        <v>35</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H73" t="s">
+        <v>36</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H76" t="s">
+        <v>37</v>
+      </c>
+      <c r="I76" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H86" t="s">
+        <v>90</v>
+      </c>
+      <c r="I86" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H87" t="s">
+        <v>39</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H89" t="s">
+        <v>40</v>
+      </c>
+      <c r="I89" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H90" t="s">
+        <v>41</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>19</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H91" t="s">
+        <v>42</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H92" t="s">
+        <v>43</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>19</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H93" t="s">
+        <v>44</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>19</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>19</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Revisión final editor pendiente motores M
Revisión final del guion, queda pendiente actualización de motores M
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado03/guion04/EsqueletoGuion_CN_03_04_CO.xlsx
+++ b/fuentes/contenidos/grado03/guion04/EsqueletoGuion_CN_03_04_CO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="92">
   <si>
     <t>FICHA</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>El deterioro que genera el ser humano a la fauna</t>
+  </si>
+  <si>
+    <t>Gráfica</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1672,7 +1675,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +1970,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2261,11 +2264,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2629,7 +2632,7 @@
         <v>56</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -2644,10 +2647,10 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -2665,7 +2668,7 @@
         <v>58</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -2680,10 +2683,10 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -2701,7 +2704,7 @@
         <v>59</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -2719,7 +2722,7 @@
         <v>59</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -2737,7 +2740,7 @@
         <v>59</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -2750,15 +2753,15 @@
       <c r="B26" s="8" t="s">
         <v>55</v>
       </c>
+      <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>49</v>
-      </c>
+      <c r="E26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2771,12 +2774,13 @@
       <c r="D27" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="F27" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2789,7 +2793,7 @@
         <v>59</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>49</v>
@@ -2809,13 +2813,7 @@
         <v>62</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H29" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2825,11 +2823,20 @@
       <c r="B30" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>49</v>
+      <c r="D30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2843,7 +2850,7 @@
         <v>63</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2854,16 +2861,10 @@
         <v>55</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H32" t="s">
-        <v>30</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2871,10 +2872,19 @@
         <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H33" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2885,7 +2895,7 @@
         <v>64</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2895,11 +2905,8 @@
       <c r="B35" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>49</v>
+      <c r="C35" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2913,7 +2920,7 @@
         <v>31</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2927,13 +2934,7 @@
         <v>31</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H37" t="s">
-        <v>31</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2944,10 +2945,16 @@
         <v>64</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="H38" t="s">
+        <v>31</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2961,7 +2968,7 @@
         <v>65</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2975,7 +2982,7 @@
         <v>65</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2986,10 +2993,10 @@
         <v>64</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3002,10 +3009,7 @@
       <c r="D42" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3020,7 +3024,7 @@
         <v>66</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>49</v>
@@ -3037,7 +3041,7 @@
         <v>66</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>49</v>
@@ -3057,7 +3061,7 @@
         <v>68</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3068,10 +3072,13 @@
         <v>64</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>49</v>
+        <v>66</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3085,7 +3092,7 @@
         <v>69</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3096,16 +3103,10 @@
         <v>64</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H48" t="s">
-        <v>32</v>
-      </c>
-      <c r="I48" s="9" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3113,9 +3114,12 @@
         <v>19</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3124,10 +3128,19 @@
         <v>19</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H50" t="s">
+        <v>32</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3148,11 +3161,8 @@
       <c r="B52" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>49</v>
+      <c r="C52" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3162,13 +3172,7 @@
       <c r="B53" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3182,11 +3186,8 @@
       <c r="D54" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>50</v>
+      <c r="E54" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3203,7 +3204,7 @@
         <v>72</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3214,10 +3215,13 @@
         <v>70</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>49</v>
+        <v>71</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3228,10 +3232,13 @@
         <v>70</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3242,7 +3249,7 @@
         <v>70</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>49</v>
@@ -3256,13 +3263,10 @@
         <v>70</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>49</v>
+        <v>73</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3275,10 +3279,7 @@
       <c r="D60" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G60" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3293,7 +3294,7 @@
         <v>74</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>49</v>
@@ -3310,16 +3311,10 @@
         <v>74</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H62" t="s">
-        <v>33</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3330,9 +3325,12 @@
         <v>70</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E63" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G63" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3344,10 +3342,19 @@
         <v>70</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>50</v>
+        <v>74</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H64" t="s">
+        <v>33</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3358,16 +3365,10 @@
         <v>70</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H65" t="s">
-        <v>34</v>
-      </c>
-      <c r="I65" s="9" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3375,10 +3376,13 @@
         <v>19</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3386,10 +3390,19 @@
         <v>19</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>50</v>
+        <v>70</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H67" t="s">
+        <v>34</v>
+      </c>
+      <c r="I67" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3399,10 +3412,7 @@
       <c r="B68" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E68" s="3" t="s">
+      <c r="C68" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3413,17 +3423,8 @@
       <c r="B69" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H69" t="s">
-        <v>35</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>27</v>
+      <c r="C69" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3434,7 +3435,7 @@
         <v>79</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>49</v>
@@ -3448,10 +3449,16 @@
         <v>79</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="H71" t="s">
+        <v>35</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3479,13 +3486,7 @@
         <v>81</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H73" t="s">
-        <v>36</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3496,7 +3497,7 @@
         <v>79</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>49</v>
@@ -3510,10 +3511,16 @@
         <v>79</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="H75" t="s">
+        <v>36</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3524,16 +3531,10 @@
         <v>79</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H76" t="s">
-        <v>37</v>
-      </c>
-      <c r="I76" s="9" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3541,10 +3542,13 @@
         <v>19</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>49</v>
+        <v>79</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3552,10 +3556,19 @@
         <v>19</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>50</v>
+        <v>79</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H78" t="s">
+        <v>37</v>
+      </c>
+      <c r="I78" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3566,7 +3579,7 @@
         <v>83</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3576,11 +3589,8 @@
       <c r="B80" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>49</v>
+      <c r="C80" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3590,11 +3600,8 @@
       <c r="B81" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>50</v>
+      <c r="C81" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3619,10 +3626,10 @@
         <v>83</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3633,10 +3640,10 @@
         <v>83</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -3664,13 +3671,7 @@
         <v>38</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H86" t="s">
-        <v>90</v>
-      </c>
-      <c r="I86" s="5" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3684,13 +3685,7 @@
         <v>38</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H87" t="s">
-        <v>39</v>
-      </c>
-      <c r="I87" s="5" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3701,10 +3696,16 @@
         <v>83</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="H88" t="s">
+        <v>90</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3715,15 +3716,15 @@
         <v>83</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>53</v>
       </c>
       <c r="H89" t="s">
-        <v>40</v>
-      </c>
-      <c r="I89" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I89" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3732,16 +3733,13 @@
         <v>19</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H90" t="s">
-        <v>41</v>
-      </c>
-      <c r="I90" s="5" t="s">
-        <v>27</v>
+        <v>83</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3749,15 +3747,18 @@
         <v>19</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C91" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>53</v>
       </c>
       <c r="H91" t="s">
-        <v>42</v>
-      </c>
-      <c r="I91" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I91" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3772,7 +3773,7 @@
         <v>53</v>
       </c>
       <c r="H92" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I92" s="5" t="s">
         <v>27</v>
@@ -3789,7 +3790,7 @@
         <v>53</v>
       </c>
       <c r="H93" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I93" s="5" t="s">
         <v>27</v>
@@ -3800,10 +3801,13 @@
         <v>19</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>88</v>
+        <v>53</v>
+      </c>
+      <c r="H94" t="s">
+        <v>43</v>
       </c>
       <c r="I94" s="5" t="s">
         <v>27</v>
@@ -3814,12 +3818,43 @@
         <v>19</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H95" t="s">
+        <v>44</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>19</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C96" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>19</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I95" s="5" t="s">
+      <c r="I97" s="5" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>